<commit_message>
Add installment reminder template 5197 with correct 5-variable format
</commit_message>
<xml_diff>
--- a/Fast2SMS WhatsApp_04Sep.xlsx
+++ b/Fast2SMS WhatsApp_04Sep.xlsx
@@ -1,21 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11008"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaditya/chords_crm/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E98BD82-F7BE-E94C-9CF9-0425D100B6E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="6620" yWindow="1740" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="WhatsApp Templates API" sheetId="1" r:id="rId4"/>
+    <sheet name="WhatsApp Templates API" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1" forceFullCalc="1"/>
+  <calcPr calcId="191029" forceFullCalc="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>message_id</t>
   </si>
@@ -101,18 +118,32 @@
 {Var6}
 🎶 Keep practicing and let your musical journey flourish! | BUTTON: Call us (PHONE_NUMBER) - +917981585309</t>
   </si>
+  <si>
+    <t>installment_payment</t>
+  </si>
+  <si>
+    <t>Var1|Var2|Var3|Var4|Var5</t>
+  </si>
+  <si>
+    <t>https://www.fast2sms.com/dev/whatsapp?authorization=&lt;YOUR_API_KEY&gt;&amp;message_id=5197&amp;numbers=&lt;MOBILE_NUMBER&gt;&amp;variables_values=Var1|Var2|Var3|Var4|Var5</t>
+  </si>
+  <si>
+    <t>HEADER: CHORDS MUSIC ACADEMY | BODY: Dear {Var1},
+INSTALLMENT REMINDER
+• Amount: ₹{Var2}
+• Due Date: {Var3}
+• Package: {Var4}
+• Expires: {Var5}
+Pay now to continue your musical journey.
+📞 7981585309 | BUTTON: Call Us (PHONE_NUMBER) - +917981585309</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -139,13 +170,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -435,19 +474,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:J3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="24.83203125" customWidth="1"/>
+    <col min="3" max="3" width="36" customWidth="1"/>
+    <col min="9" max="9" width="133" customWidth="1"/>
+    <col min="10" max="10" width="77.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -479,7 +521,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>5170</v>
       </c>
@@ -511,7 +553,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>5171</v>
       </c>
@@ -543,18 +585,40 @@
         <v>22</v>
       </c>
     </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>5197</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
-  <tableParts count="0"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>